<commit_message>
fix requairements vertion for stable working
</commit_message>
<xml_diff>
--- a/app/data/HallList-good.xlsx
+++ b/app/data/HallList-good.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgijmamarin/Desktop/Figaro_bot/Figaro_bot-2/Figaro/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98DC609-A44D-834E-BA00-D9FB7C4FACC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B8E547-1019-C046-B3BE-6A14CDB9741A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7080" yWindow="-20080" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -477,7 +478,7 @@
         <v>16</v>
       </c>
       <c r="D2">
-        <v>700</v>
+        <v>743</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -494,7 +495,7 @@
         <v>14</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -511,7 +512,7 @@
         <v>15</v>
       </c>
       <c r="D4">
-        <v>400</v>
+        <v>340</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -528,7 +529,7 @@
         <v>14</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -545,7 +546,7 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>157</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -562,7 +563,7 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>1400</v>
+        <v>1620</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -579,7 +580,7 @@
         <v>14</v>
       </c>
       <c r="D8">
-        <v>900</v>
+        <v>650</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -596,7 +597,7 @@
         <v>12</v>
       </c>
       <c r="D9">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E9">
         <v>0</v>

</xml_diff>

<commit_message>
add data model OffProgram and upload at data_loader
</commit_message>
<xml_diff>
--- a/app/data/HallList-good.xlsx
+++ b/app/data/HallList-good.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgijmamarin/Desktop/Figaro_bot/Figaro_bot-2/Figaro/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B8E547-1019-C046-B3BE-6A14CDB9741A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663D66BF-C0BD-F449-A5CB-D690ABE94C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>HallName</t>
   </si>
@@ -76,6 +75,27 @@
   </si>
   <si>
     <t>Seats</t>
+  </si>
+  <si>
+    <t>ул. К. Либкнехта, 48</t>
+  </si>
+  <si>
+    <t>ул. Я. Свердлова, 30</t>
+  </si>
+  <si>
+    <t>ул. Пролетарская, 18</t>
+  </si>
+  <si>
+    <t>ул. К. Либкнехта, 38а</t>
+  </si>
+  <si>
+    <t>ул. Первомайская, 22</t>
+  </si>
+  <si>
+    <t>ул. Первомайская, 9</t>
+  </si>
+  <si>
+    <t>Инфоцентр</t>
   </si>
 </sst>
 </file>
@@ -105,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -128,13 +148,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -439,15 +473,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -477,6 +512,9 @@
       <c r="B2">
         <v>16</v>
       </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
       <c r="D2">
         <v>743</v>
       </c>
@@ -494,6 +532,9 @@
       <c r="B3">
         <v>14</v>
       </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
       <c r="D3">
         <v>120</v>
       </c>
@@ -511,6 +552,9 @@
       <c r="B4">
         <v>15</v>
       </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
       <c r="D4">
         <v>340</v>
       </c>
@@ -528,6 +572,9 @@
       <c r="B5">
         <v>14</v>
       </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
       <c r="D5">
         <v>150</v>
       </c>
@@ -545,6 +592,9 @@
       <c r="B6">
         <v>12</v>
       </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
       <c r="D6">
         <v>157</v>
       </c>
@@ -562,6 +612,9 @@
       <c r="B7">
         <v>3</v>
       </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
       <c r="D7">
         <v>1620</v>
       </c>
@@ -579,6 +632,9 @@
       <c r="B8">
         <v>14</v>
       </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
       <c r="D8">
         <v>650</v>
       </c>
@@ -596,6 +652,9 @@
       <c r="B9">
         <v>12</v>
       </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
       <c r="D9">
         <v>145</v>
       </c>
@@ -603,6 +662,26 @@
         <v>0</v>
       </c>
       <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>0</v>
       </c>
     </row>

</xml_diff>